<commit_message>
aproximação maior dos valores do certificado 30/07/2025
</commit_message>
<xml_diff>
--- a/SAN-038-25-09_CORRIGIDO.xlsx
+++ b/SAN-038-25-09_CORRIGIDO.xlsx
@@ -7285,12 +7285,12 @@
     </row>
     <row r="54" ht="13.5" customHeight="1" thickBot="1">
       <c r="C54" s="162" t="n">
-        <v>16924</v>
+        <v>16830</v>
       </c>
       <c r="D54" s="668" t="n"/>
       <c r="E54" s="669" t="n"/>
       <c r="F54" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G54" s="668" t="n"/>
       <c r="H54" s="669" t="n"/>
@@ -7307,7 +7307,7 @@
       <c r="M54" s="666" t="n"/>
       <c r="N54" s="667" t="n"/>
       <c r="O54" s="162" t="n">
-        <v>3387.723792899408</v>
+        <v>3368.850810946746</v>
       </c>
       <c r="P54" s="668" t="n"/>
       <c r="Q54" s="669" t="n"/>
@@ -7357,12 +7357,12 @@
     </row>
     <row r="55" ht="13.5" customHeight="1" thickBot="1">
       <c r="C55" s="162" t="n">
-        <v>16999</v>
+        <v>16904</v>
       </c>
       <c r="D55" s="668" t="n"/>
       <c r="E55" s="669" t="n"/>
       <c r="F55" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G55" s="668" t="n"/>
       <c r="H55" s="669" t="n"/>
@@ -7379,7 +7379,7 @@
       <c r="M55" s="666" t="n"/>
       <c r="N55" s="667" t="n"/>
       <c r="O55" s="162" t="n">
-        <v>3397.141676855895</v>
+        <v>3378.216227947598</v>
       </c>
       <c r="P55" s="668" t="n"/>
       <c r="Q55" s="669" t="n"/>
@@ -7431,12 +7431,12 @@
     </row>
     <row r="56" ht="13.5" customHeight="1" thickBot="1">
       <c r="C56" s="162" t="n">
-        <v>17044</v>
+        <v>16949</v>
       </c>
       <c r="D56" s="668" t="n"/>
       <c r="E56" s="669" t="n"/>
       <c r="F56" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G56" s="668" t="n"/>
       <c r="H56" s="669" t="n"/>
@@ -7453,7 +7453,7 @@
       <c r="M56" s="666" t="n"/>
       <c r="N56" s="667" t="n"/>
       <c r="O56" s="162" t="n">
-        <v>3398.468452249135</v>
+        <v>3379.535611885813</v>
       </c>
       <c r="P56" s="668" t="n"/>
       <c r="Q56" s="669" t="n"/>
@@ -7909,12 +7909,12 @@
     </row>
     <row r="63" ht="13.5" customHeight="1" thickBot="1">
       <c r="C63" s="162" t="n">
-        <v>28470</v>
+        <v>28311</v>
       </c>
       <c r="D63" s="668" t="n"/>
       <c r="E63" s="669" t="n"/>
       <c r="F63" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G63" s="668" t="n"/>
       <c r="H63" s="669" t="n"/>
@@ -7931,7 +7931,7 @@
       <c r="M63" s="666" t="n"/>
       <c r="N63" s="667" t="n"/>
       <c r="O63" s="162" t="n">
-        <v>5707.414911801242</v>
+        <v>5675.61894931677</v>
       </c>
       <c r="P63" s="668" t="n"/>
       <c r="Q63" s="669" t="n"/>
@@ -7978,12 +7978,12 @@
     </row>
     <row r="64" ht="13.5" customHeight="1" thickBot="1">
       <c r="C64" s="162" t="n">
-        <v>28525</v>
+        <v>28366</v>
       </c>
       <c r="D64" s="668" t="n"/>
       <c r="E64" s="669" t="n"/>
       <c r="F64" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G64" s="668" t="n"/>
       <c r="H64" s="669" t="n"/>
@@ -8000,7 +8000,7 @@
       <c r="M64" s="666" t="n"/>
       <c r="N64" s="667" t="n"/>
       <c r="O64" s="162" t="n">
-        <v>5719.902099547511</v>
+        <v>5688.036571040724</v>
       </c>
       <c r="P64" s="668" t="n"/>
       <c r="Q64" s="669" t="n"/>
@@ -8045,12 +8045,12 @@
     </row>
     <row r="65" ht="13.5" customHeight="1" thickBot="1">
       <c r="C65" s="162" t="n">
-        <v>28561</v>
+        <v>28402</v>
       </c>
       <c r="D65" s="668" t="n"/>
       <c r="E65" s="669" t="n"/>
       <c r="F65" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G65" s="668" t="n"/>
       <c r="H65" s="669" t="n"/>
@@ -8067,7 +8067,7 @@
       <c r="M65" s="666" t="n"/>
       <c r="N65" s="667" t="n"/>
       <c r="O65" s="162" t="n">
-        <v>5726.312545551601</v>
+        <v>5694.411304501779</v>
       </c>
       <c r="P65" s="668" t="n"/>
       <c r="Q65" s="669" t="n"/>
@@ -8473,12 +8473,12 @@
     </row>
     <row r="72" ht="13.5" customHeight="1" thickBot="1">
       <c r="C72" s="162" t="n">
-        <v>56578</v>
+        <v>56263</v>
       </c>
       <c r="D72" s="668" t="n"/>
       <c r="E72" s="669" t="n"/>
       <c r="F72" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G72" s="668" t="n"/>
       <c r="H72" s="669" t="n"/>
@@ -8495,7 +8495,7 @@
       <c r="M72" s="666" t="n"/>
       <c r="N72" s="667" t="n"/>
       <c r="O72" s="162" t="n">
-        <v>11301.08972340425</v>
+        <v>11238.13144361702</v>
       </c>
       <c r="P72" s="668" t="n"/>
       <c r="Q72" s="669" t="n"/>
@@ -8531,12 +8531,12 @@
     </row>
     <row r="73" ht="13.5" customHeight="1" thickBot="1">
       <c r="C73" s="162" t="n">
-        <v>56703</v>
+        <v>56387</v>
       </c>
       <c r="D73" s="668" t="n"/>
       <c r="E73" s="669" t="n"/>
       <c r="F73" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G73" s="668" t="n"/>
       <c r="H73" s="669" t="n"/>
@@ -8553,7 +8553,7 @@
       <c r="M73" s="666" t="n"/>
       <c r="N73" s="667" t="n"/>
       <c r="O73" s="162" t="n">
-        <v>11338.40240447761</v>
+        <v>11275.23625604478</v>
       </c>
       <c r="P73" s="668" t="n"/>
       <c r="Q73" s="669" t="n"/>
@@ -8589,12 +8589,12 @@
     </row>
     <row r="74" ht="13.5" customHeight="1" thickBot="1">
       <c r="C74" s="162" t="n">
-        <v>56792</v>
+        <v>56476</v>
       </c>
       <c r="D74" s="668" t="n"/>
       <c r="E74" s="669" t="n"/>
       <c r="F74" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G74" s="668" t="n"/>
       <c r="H74" s="669" t="n"/>
@@ -8611,7 +8611,7 @@
       <c r="M74" s="666" t="n"/>
       <c r="N74" s="667" t="n"/>
       <c r="O74" s="162" t="n">
-        <v>11384.06033065134</v>
+        <v>11320.63982227969</v>
       </c>
       <c r="P74" s="668" t="n"/>
       <c r="Q74" s="669" t="n"/>
@@ -8968,12 +8968,12 @@
     </row>
     <row r="81" ht="13.5" customHeight="1" thickBot="1">
       <c r="C81" s="162" t="n">
-        <v>83760</v>
+        <v>83293</v>
       </c>
       <c r="D81" s="668" t="n"/>
       <c r="E81" s="669" t="n"/>
       <c r="F81" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G81" s="668" t="n"/>
       <c r="H81" s="669" t="n"/>
@@ -8990,7 +8990,7 @@
       <c r="M81" s="666" t="n"/>
       <c r="N81" s="667" t="n"/>
       <c r="O81" s="162" t="n">
-        <v>16730.583574375</v>
+        <v>16637.37762809375</v>
       </c>
       <c r="P81" s="668" t="n"/>
       <c r="Q81" s="669" t="n"/>
@@ -9026,12 +9026,12 @@
     </row>
     <row r="82" ht="13.5" customHeight="1" thickBot="1">
       <c r="C82" s="162" t="n">
-        <v>84033</v>
+        <v>83565</v>
       </c>
       <c r="D82" s="668" t="n"/>
       <c r="E82" s="669" t="n"/>
       <c r="F82" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G82" s="668" t="n"/>
       <c r="H82" s="669" t="n"/>
@@ -9048,7 +9048,7 @@
       <c r="M82" s="666" t="n"/>
       <c r="N82" s="667" t="n"/>
       <c r="O82" s="162" t="n">
-        <v>16829.24954590909</v>
+        <v>16735.49393229546</v>
       </c>
       <c r="P82" s="668" t="n"/>
       <c r="Q82" s="669" t="n"/>
@@ -9084,12 +9084,12 @@
     </row>
     <row r="83" ht="13.5" customHeight="1" thickBot="1">
       <c r="C83" s="162" t="n">
-        <v>84201</v>
+        <v>83732</v>
       </c>
       <c r="D83" s="668" t="n"/>
       <c r="E83" s="669" t="n"/>
       <c r="F83" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G83" s="668" t="n"/>
       <c r="H83" s="669" t="n"/>
@@ -9106,7 +9106,7 @@
       <c r="M83" s="666" t="n"/>
       <c r="N83" s="667" t="n"/>
       <c r="O83" s="162" t="n">
-        <v>16859.11318321429</v>
+        <v>16765.19119951786</v>
       </c>
       <c r="P83" s="668" t="n"/>
       <c r="Q83" s="669" t="n"/>
@@ -9467,12 +9467,12 @@
     </row>
     <row r="90" ht="13.5" customHeight="1" thickBot="1">
       <c r="C90" s="162" t="n">
-        <v>112430</v>
+        <v>111804</v>
       </c>
       <c r="D90" s="668" t="n"/>
       <c r="E90" s="669" t="n"/>
       <c r="F90" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G90" s="668" t="n"/>
       <c r="H90" s="669" t="n"/>
@@ -9489,7 +9489,7 @@
       <c r="M90" s="666" t="n"/>
       <c r="N90" s="667" t="n"/>
       <c r="O90" s="162" t="n">
-        <v>22475.56571925926</v>
+        <v>22350.35452374074</v>
       </c>
       <c r="P90" s="668" t="n"/>
       <c r="Q90" s="669" t="n"/>
@@ -9525,12 +9525,12 @@
     </row>
     <row r="91" ht="13.5" customHeight="1" thickBot="1">
       <c r="C91" s="162" t="n">
-        <v>112127</v>
+        <v>111503</v>
       </c>
       <c r="D91" s="668" t="n"/>
       <c r="E91" s="669" t="n"/>
       <c r="F91" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G91" s="668" t="n"/>
       <c r="H91" s="669" t="n"/>
@@ -9547,7 +9547,7 @@
       <c r="M91" s="666" t="n"/>
       <c r="N91" s="667" t="n"/>
       <c r="O91" s="162" t="n">
-        <v>22450.53262040816</v>
+        <v>22325.46088408163</v>
       </c>
       <c r="P91" s="668" t="n"/>
       <c r="Q91" s="669" t="n"/>
@@ -9583,12 +9583,12 @@
     </row>
     <row r="92" ht="13.5" customHeight="1" thickBot="1">
       <c r="C92" s="162" t="n">
-        <v>112369</v>
+        <v>111743</v>
       </c>
       <c r="D92" s="668" t="n"/>
       <c r="E92" s="669" t="n"/>
       <c r="F92" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G92" s="668" t="n"/>
       <c r="H92" s="669" t="n"/>
@@ -9605,7 +9605,7 @@
       <c r="M92" s="666" t="n"/>
       <c r="N92" s="667" t="n"/>
       <c r="O92" s="162" t="n">
-        <v>22531.53528242188</v>
+        <v>22406.01228091797</v>
       </c>
       <c r="P92" s="668" t="n"/>
       <c r="Q92" s="669" t="n"/>
@@ -9957,12 +9957,12 @@
     </row>
     <row r="99" ht="13.5" customHeight="1" thickBot="1">
       <c r="C99" s="162" t="n">
-        <v>16957</v>
+        <v>16863</v>
       </c>
       <c r="D99" s="668" t="n"/>
       <c r="E99" s="669" t="n"/>
       <c r="F99" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G99" s="668" t="n"/>
       <c r="H99" s="669" t="n"/>
@@ -9979,7 +9979,7 @@
       <c r="M99" s="666" t="n"/>
       <c r="N99" s="667" t="n"/>
       <c r="O99" s="162" t="n">
-        <v>3391.391018518519</v>
+        <v>3372.497606481481</v>
       </c>
       <c r="P99" s="668" t="n"/>
       <c r="Q99" s="669" t="n"/>
@@ -10015,12 +10015,12 @@
     </row>
     <row r="100" ht="13.5" customHeight="1" thickBot="1">
       <c r="C100" s="162" t="n">
-        <v>16905</v>
+        <v>16811</v>
       </c>
       <c r="D100" s="668" t="n"/>
       <c r="E100" s="669" t="n"/>
       <c r="F100" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G100" s="668" t="n"/>
       <c r="H100" s="669" t="n"/>
@@ -10037,7 +10037,7 @@
       <c r="M100" s="666" t="n"/>
       <c r="N100" s="667" t="n"/>
       <c r="O100" s="162" t="n">
-        <v>3379.158684</v>
+        <v>3360.3334182</v>
       </c>
       <c r="P100" s="668" t="n"/>
       <c r="Q100" s="669" t="n"/>
@@ -10073,12 +10073,12 @@
     </row>
     <row r="101" ht="13.5" customHeight="1" thickBot="1">
       <c r="C101" s="162" t="n">
-        <v>16933</v>
+        <v>16838</v>
       </c>
       <c r="D101" s="668" t="n"/>
       <c r="E101" s="669" t="n"/>
       <c r="F101" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G101" s="668" t="n"/>
       <c r="H101" s="669" t="n"/>
@@ -10095,7 +10095,7 @@
       <c r="M101" s="666" t="n"/>
       <c r="N101" s="667" t="n"/>
       <c r="O101" s="162" t="n">
-        <v>3386.143530322581</v>
+        <v>3367.279352</v>
       </c>
       <c r="P101" s="668" t="n"/>
       <c r="Q101" s="669" t="n"/>
@@ -10447,12 +10447,12 @@
     </row>
     <row r="108" ht="13.5" customHeight="1" thickBot="1">
       <c r="C108" s="162" t="n">
-        <v>56424</v>
+        <v>56110</v>
       </c>
       <c r="D108" s="668" t="n"/>
       <c r="E108" s="669" t="n"/>
       <c r="F108" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G108" s="668" t="n"/>
       <c r="H108" s="669" t="n"/>
@@ -10469,7 +10469,7 @@
       <c r="M108" s="666" t="n"/>
       <c r="N108" s="667" t="n"/>
       <c r="O108" s="162" t="n">
-        <v>11277.47779098039</v>
+        <v>11214.65105307843</v>
       </c>
       <c r="P108" s="668" t="n"/>
       <c r="Q108" s="669" t="n"/>
@@ -10505,12 +10505,12 @@
     </row>
     <row r="109" ht="13.5" customHeight="1" thickBot="1">
       <c r="C109" s="162" t="n">
-        <v>56518</v>
+        <v>56203</v>
       </c>
       <c r="D109" s="668" t="n"/>
       <c r="E109" s="669" t="n"/>
       <c r="F109" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G109" s="668" t="n"/>
       <c r="H109" s="669" t="n"/>
@@ -10527,7 +10527,7 @@
       <c r="M109" s="666" t="n"/>
       <c r="N109" s="667" t="n"/>
       <c r="O109" s="162" t="n">
-        <v>11296.10817746032</v>
+        <v>11233.1776498254</v>
       </c>
       <c r="P109" s="668" t="n"/>
       <c r="Q109" s="669" t="n"/>
@@ -10563,12 +10563,12 @@
     </row>
     <row r="110" ht="13.5" customHeight="1" thickBot="1">
       <c r="C110" s="162" t="n">
-        <v>56577</v>
+        <v>56231</v>
       </c>
       <c r="D110" s="668" t="n"/>
       <c r="E110" s="669" t="n"/>
       <c r="F110" s="162" t="n">
-        <v>360.1</v>
+        <v>357.895</v>
       </c>
       <c r="G110" s="668" t="n"/>
       <c r="H110" s="669" t="n"/>
@@ -10585,7 +10585,7 @@
       <c r="M110" s="666" t="n"/>
       <c r="N110" s="667" t="n"/>
       <c r="O110" s="162" t="n">
-        <v>11318.41641146667</v>
+        <v>11249.11036262667</v>
       </c>
       <c r="P110" s="668" t="n"/>
       <c r="Q110" s="669" t="n"/>
@@ -10924,12 +10924,12 @@
     </row>
     <row r="117" ht="13.5" customHeight="1" thickBot="1">
       <c r="C117" s="162" t="n">
-        <v>112811</v>
+        <v>112182</v>
       </c>
       <c r="D117" s="668" t="n"/>
       <c r="E117" s="669" t="n"/>
       <c r="F117" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G117" s="668" t="n"/>
       <c r="H117" s="669" t="n"/>
@@ -10946,7 +10946,7 @@
       <c r="M117" s="666" t="n"/>
       <c r="N117" s="667" t="n"/>
       <c r="O117" s="162" t="n">
-        <v>22592.16749631579</v>
+        <v>22466.30671323684</v>
       </c>
       <c r="P117" s="668" t="n"/>
       <c r="Q117" s="669" t="n"/>
@@ -10984,12 +10984,12 @@
     </row>
     <row r="118" ht="13.5" customHeight="1" thickBot="1">
       <c r="C118" s="162" t="n">
-        <v>112954</v>
+        <v>112325</v>
       </c>
       <c r="D118" s="668" t="n"/>
       <c r="E118" s="669" t="n"/>
       <c r="F118" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G118" s="668" t="n"/>
       <c r="H118" s="669" t="n"/>
@@ -11006,7 +11006,7 @@
       <c r="M118" s="666" t="n"/>
       <c r="N118" s="667" t="n"/>
       <c r="O118" s="162" t="n">
-        <v>22599.9095939394</v>
+        <v>22474.00567969697</v>
       </c>
       <c r="P118" s="668" t="n"/>
       <c r="Q118" s="669" t="n"/>
@@ -11044,12 +11044,12 @@
     </row>
     <row r="119" ht="13.5" customHeight="1" thickBot="1">
       <c r="C119" s="162" t="n">
-        <v>113077</v>
+        <v>112447</v>
       </c>
       <c r="D119" s="668" t="n"/>
       <c r="E119" s="669" t="n"/>
       <c r="F119" s="162" t="n">
-        <v>359.9</v>
+        <v>357.895</v>
       </c>
       <c r="G119" s="668" t="n"/>
       <c r="H119" s="669" t="n"/>
@@ -11066,7 +11066,7 @@
       <c r="M119" s="666" t="n"/>
       <c r="N119" s="667" t="n"/>
       <c r="O119" s="162" t="n">
-        <v>22625.31385670103</v>
+        <v>22499.26841551546</v>
       </c>
       <c r="P119" s="668" t="n"/>
       <c r="Q119" s="669" t="n"/>

</xml_diff>